<commit_message>
remove outliers should be fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\stats_standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68761DE0-16F8-49C4-8A79-585ACF7AC63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A787D3BD-9C09-4E7E-96C5-A4F1B16D0A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-14150" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{A3113F25-9CDE-41D3-828A-815A98394DB0}"/>
+    <workbookView xWindow="-38510" yWindow="-14150" windowWidth="38620" windowHeight="21100" xr2:uid="{A3113F25-9CDE-41D3-828A-815A98394DB0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB65F0B4-8D4D-4F81-9A8D-3EABB2BB1A50}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,7 +490,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -502,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDB0BCE-1A4F-4D7F-8E79-ACB7AD078578}">
   <dimension ref="A3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>